<commit_message>
Creating Test Case and executing it on 10 different nodes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
   <si>
     <t>TestCases</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Kalim Neon</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -422,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,12 +482,12 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -491,8 +500,11 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -505,10 +517,13 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -519,75 +534,214 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrating ExtentReport for parallel tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>TestCases</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
@@ -79,15 +76,6 @@
   </si>
   <si>
     <t>Rupee</t>
-  </si>
-  <si>
-    <t>Vasya Vasiliev</t>
-  </si>
-  <si>
-    <t>Test Testov</t>
-  </si>
-  <si>
-    <t>Kalim Neon</t>
   </si>
   <si>
     <t>browser</t>
@@ -471,10 +459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,16 +480,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -509,16 +497,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -526,67 +514,35 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -594,16 +550,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -611,138 +564,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addying more test steps
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>TestCases</t>
   </si>
@@ -48,33 +48,21 @@
     <t>Ivanov</t>
   </si>
   <si>
-    <t>e3r4t5</t>
-  </si>
-  <si>
     <t>Petr</t>
   </si>
   <si>
     <t>Petrov</t>
   </si>
   <si>
-    <t>2af4g5</t>
-  </si>
-  <si>
     <t>customer</t>
   </si>
   <si>
     <t>currency</t>
   </si>
   <si>
-    <t>Ivan Ivanov</t>
-  </si>
-  <si>
     <t>Dollar</t>
   </si>
   <si>
-    <t>Petr Petrov</t>
-  </si>
-  <si>
     <t>Rupee</t>
   </si>
   <si>
@@ -85,6 +73,30 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>Vasya</t>
+  </si>
+  <si>
+    <t>Vasiliev</t>
+  </si>
+  <si>
+    <t>Hermoine Granger</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Ron Weasly</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>dhfgh</t>
+  </si>
+  <si>
+    <t>fghfhf</t>
   </si>
 </sst>
 </file>
@@ -459,10 +471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,10 +515,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -514,49 +526,52 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -564,13 +579,41 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>